<commit_message>
V4.12.1.90 - More work on device editor
</commit_message>
<xml_diff>
--- a/net.sourceforge.usbdm.deviceEditor/Extracted/Pages from K20P64M50SF0RM.xlsx
+++ b/net.sourceforge.usbdm.deviceEditor/Extracted/Pages from K20P64M50SF0RM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podonoghue\Documents\Development\USBDM\usbdm-eclipse-plugins\CreateCppStationeryByPin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podonoghue\Documents\Development\USBDM\usbdm-eclipse-plugins\net.sourceforge.usbdm.deviceEditor\Extracted\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="20" windowWidth="18960" windowHeight="11330"/>
+    <workbookView xWindow="120" yWindow="400" windowWidth="18960" windowHeight="11330"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1546,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49:G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="12.5" x14ac:dyDescent="0.3"/>
@@ -1557,13 +1557,7 @@
     <col min="3" max="3" width="15.8984375" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.59765625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.09765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="29.09765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.09765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.59765625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.69921875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="13" width="9.59765625" style="7" customWidth="1"/>
     <col min="14" max="14" width="10.69921875" style="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.3984375" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.296875" style="4" bestFit="1" customWidth="1"/>
@@ -1628,27 +1622,39 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>265</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D2" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="O2" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="9">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="R2" s="10" t="s">
         <v>266</v>
@@ -1659,219 +1665,157 @@
         <v>265</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="8"/>
+        <v>209</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="D3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="O3" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="Q3" s="9">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>265</v>
-      </c>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="1"/>
+      <c r="D4" s="8"/>
       <c r="F4" s="8"/>
       <c r="O4" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="Q4" s="9">
-        <v>9</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="R4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="1"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="O5" s="4">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="9">
-        <v>11</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="R5" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>223</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="E6" s="1"/>
+      <c r="D6" s="8"/>
       <c r="F6" s="8"/>
       <c r="O6" s="4">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="Q6" s="9">
-        <v>18</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="R6" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="1"/>
+      <c r="D7" s="8"/>
       <c r="F7" s="8"/>
       <c r="O7" s="4">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="Q7" s="9">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="R7" s="9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>83</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="O8" s="4">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="Q8" s="9">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="R8" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>90</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="O9" s="4">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="Q9" s="9">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="R9" s="9">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1879,86 +1823,51 @@
         <v>265</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>96</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="8"/>
       <c r="O10" s="4">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="Q10" s="9">
-        <v>24</v>
-      </c>
-      <c r="R10" s="9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>265</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>330</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
       <c r="O11" s="4">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="Q11" s="9">
-        <v>25</v>
-      </c>
-      <c r="R11" s="9">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="R11" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1966,41 +1875,25 @@
         <v>265</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>272</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>105</v>
-      </c>
+      <c r="F12" s="8"/>
       <c r="O12" s="4">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="Q12" s="9">
-        <v>26</v>
-      </c>
-      <c r="R12" s="9">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="R12" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2008,246 +1901,133 @@
         <v>265</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>52</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>332</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="8"/>
       <c r="O13" s="4">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>106</v>
+        <v>60</v>
       </c>
       <c r="Q13" s="9">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="R13" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>265</v>
-      </c>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>5</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
       <c r="O14" s="4">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="Q14" s="9">
-        <v>28</v>
-      </c>
-      <c r="R14" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="R14" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
       <c r="O15" s="4">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="P15" s="6" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="Q15" s="9">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="R15" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>265</v>
-      </c>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="I16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="O16" s="4">
+        <v>15</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>15</v>
+      </c>
+      <c r="R16" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="O17" s="4">
+        <v>16</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>16</v>
+      </c>
+      <c r="R17" s="9">
         <v>8</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="O16" s="4">
-        <v>32</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q16" s="9">
-        <v>32</v>
-      </c>
-      <c r="R16" s="9">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="O18" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="O17" s="4">
-        <v>33</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q17" s="9">
-        <v>33</v>
-      </c>
-      <c r="R17" s="9">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O18" s="4">
-        <v>35</v>
-      </c>
       <c r="P18" s="6" t="s">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="Q18" s="9">
-        <v>35</v>
-      </c>
-      <c r="R18" s="9">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="R18" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -2255,87 +2035,46 @@
         <v>265</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="8"/>
       <c r="O19" s="4">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="Q19" s="9">
-        <v>36</v>
-      </c>
-      <c r="R19" s="9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>13</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
       <c r="O20" s="4">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="Q20" s="9">
-        <v>37</v>
-      </c>
-      <c r="R20" s="10" t="s">
-        <v>266</v>
+        <v>19</v>
+      </c>
+      <c r="R20" s="9">
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2343,82 +2082,45 @@
         <v>265</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>14</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="8"/>
       <c r="O21" s="4">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="P21" s="6" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="Q21" s="9">
-        <v>38</v>
-      </c>
-      <c r="R21" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="R21" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>135</v>
+        <v>78</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="D22" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>137</v>
-      </c>
+      <c r="D22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="O22" s="4">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="P22" s="6" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
       <c r="Q22" s="9">
-        <v>39</v>
-      </c>
-      <c r="R22" s="10" t="s">
-        <v>266</v>
+        <v>21</v>
+      </c>
+      <c r="R22" s="9">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -2426,38 +2128,42 @@
         <v>265</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="8" t="s">
-        <v>140</v>
+        <v>81</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>237</v>
+        <v>224</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>335</v>
+        <v>82</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="O23" s="4">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
       <c r="Q23" s="9">
-        <v>40</v>
-      </c>
-      <c r="R23" s="10" t="s">
-        <v>266</v>
+        <v>22</v>
+      </c>
+      <c r="R23" s="9">
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -2465,35 +2171,46 @@
         <v>265</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C24" s="8"/>
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="D24" s="8" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>4</v>
+        <v>225</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N24" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="O24" s="4">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>141</v>
+        <v>84</v>
       </c>
       <c r="Q24" s="9">
-        <v>41</v>
-      </c>
-      <c r="R24" s="10" t="s">
-        <v>266</v>
+        <v>23</v>
+      </c>
+      <c r="R24" s="9">
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2501,35 +2218,46 @@
         <v>265</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8" t="s">
-        <v>146</v>
+        <v>92</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>239</v>
+        <v>95</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>6</v>
+        <v>230</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="O25" s="4">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="Q25" s="9">
-        <v>42</v>
-      </c>
-      <c r="R25" s="10" t="s">
-        <v>266</v>
+        <v>24</v>
+      </c>
+      <c r="R25" s="9">
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2537,40 +2265,39 @@
         <v>265</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>205</v>
+        <v>98</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="H26" s="8" t="s">
-        <v>149</v>
+        <v>231</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>331</v>
       </c>
       <c r="I26" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="O26" s="4">
+        <v>25</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>25</v>
+      </c>
+      <c r="R26" s="9">
         <v>15</v>
-      </c>
-      <c r="O26" s="4">
-        <v>43</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q26" s="9">
-        <v>43</v>
-      </c>
-      <c r="R26" s="10" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2578,46 +2305,41 @@
         <v>265</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>203</v>
+        <v>272</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="8" t="s">
+        <v>102</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>112</v>
+        <v>232</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="O27" s="4">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="Q27" s="9">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="R27" s="9">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2625,46 +2347,43 @@
         <v>265</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>204</v>
+        <v>52</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>103</v>
+        <v>3</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>332</v>
       </c>
       <c r="O28" s="4">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="Q28" s="9">
-        <v>45</v>
-      </c>
-      <c r="R28" s="9">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="R28" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2672,46 +2391,40 @@
         <v>265</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>214</v>
+        <v>110</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>280</v>
+        <v>147</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>156</v>
+        <v>38</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>156</v>
+        <v>226</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>157</v>
+        <v>226</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>4</v>
+        <v>112</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="O29" s="4">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>155</v>
+        <v>109</v>
       </c>
       <c r="Q29" s="9">
-        <v>46</v>
-      </c>
-      <c r="R29" s="9">
-        <v>24</v>
+        <v>28</v>
+      </c>
+      <c r="R29" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2719,134 +2432,82 @@
         <v>265</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>138</v>
+        <v>273</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>161</v>
+        <v>227</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="O30" s="4">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="Q30" s="9">
-        <v>49</v>
-      </c>
-      <c r="R30" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="R30" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>18</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
       <c r="O31" s="4">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="Q31" s="9">
-        <v>50</v>
-      </c>
-      <c r="R31" s="9">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>265</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="R31" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>21</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
       <c r="O32" s="4">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="Q32" s="9">
-        <v>51</v>
-      </c>
-      <c r="R32" s="9">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="R32" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2854,43 +2515,36 @@
         <v>265</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>283</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C33" s="1"/>
       <c r="D33" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>251</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E33" s="1"/>
       <c r="F33" s="8" t="s">
-        <v>170</v>
+        <v>119</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>171</v>
+        <v>228</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="O33" s="4">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="P33" s="6" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="Q33" s="9">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="R33" s="9">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -2898,75 +2552,62 @@
         <v>265</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>84</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C34" s="1"/>
       <c r="D34" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>252</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="8" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>252</v>
+        <v>229</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="O34" s="4">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="P34" s="6" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="Q34" s="9">
-        <v>53</v>
-      </c>
-      <c r="R34" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="R34" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>265</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>20</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="F35" s="8"/>
       <c r="O35" s="4">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="P35" s="6" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="Q35" s="9">
-        <v>54</v>
-      </c>
-      <c r="R35" s="10" t="s">
-        <v>266</v>
+        <v>34</v>
+      </c>
+      <c r="R35" s="9">
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -2974,34 +2615,43 @@
         <v>265</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>38</v>
+        <v>274</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>333</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>244</v>
+        <v>126</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>333</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>23</v>
+        <v>234</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="O36" s="4">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="Q36" s="9">
-        <v>55</v>
-      </c>
-      <c r="R36" s="10" t="s">
-        <v>266</v>
+        <v>35</v>
+      </c>
+      <c r="R36" s="9">
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3009,31 +2659,43 @@
         <v>265</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>218</v>
+        <v>128</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>38</v>
+        <v>275</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>245</v>
+        <v>129</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>334</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>245</v>
+        <v>235</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="O37" s="4">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="P37" s="6" t="s">
-        <v>180</v>
+        <v>127</v>
       </c>
       <c r="Q37" s="9">
-        <v>56</v>
-      </c>
-      <c r="R37" s="10" t="s">
-        <v>266</v>
+        <v>36</v>
+      </c>
+      <c r="R37" s="9">
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3041,34 +2703,40 @@
         <v>265</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>219</v>
+        <v>131</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>38</v>
+        <v>276</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>202</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>254</v>
+        <v>240</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>202</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>338</v>
+        <v>331</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="O38" s="4">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="P38" s="6" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="Q38" s="9">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="R38" s="10" t="s">
         <v>266</v>
@@ -3079,37 +2747,40 @@
         <v>265</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>339</v>
+        <v>277</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>201</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>339</v>
+        <v>241</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>201</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>340</v>
+        <v>129</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="O39" s="4">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="P39" s="6" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="Q39" s="9">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="R39" s="10" t="s">
         <v>266</v>
@@ -3120,34 +2791,35 @@
         <v>265</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>289</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C40" s="8"/>
       <c r="D40" s="8" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>19</v>
+        <v>87</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>19</v>
+        <v>236</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>185</v>
+        <v>87</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="O40" s="4">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="Q40" s="9">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="R40" s="10" t="s">
         <v>266</v>
@@ -3158,34 +2830,35 @@
         <v>265</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>290</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="C41" s="8"/>
       <c r="D41" s="8" t="s">
-        <v>38</v>
+        <v>140</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>171</v>
+        <v>94</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>188</v>
+        <v>94</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>335</v>
       </c>
       <c r="O41" s="4">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="P41" s="6" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="Q41" s="9">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="R41" s="10" t="s">
         <v>266</v>
@@ -3196,43 +2869,35 @@
         <v>265</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>291</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C42" s="8"/>
       <c r="D42" s="8" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>190</v>
+        <v>238</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>143</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>331</v>
+        <v>238</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="L42" s="8" t="s">
-        <v>137</v>
+        <v>4</v>
       </c>
       <c r="O42" s="4">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="P42" s="6" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
       <c r="Q42" s="9">
-        <v>61</v>
-      </c>
-      <c r="R42" s="9">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="R42" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -3240,46 +2905,35 @@
         <v>265</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>341</v>
+        <v>145</v>
+      </c>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>341</v>
+        <v>239</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>25</v>
+        <v>239</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="L43" s="7" t="s">
-        <v>335</v>
+        <v>6</v>
       </c>
       <c r="O43" s="4">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="P43" s="6" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="Q43" s="9">
-        <v>62</v>
-      </c>
-      <c r="R43" s="9">
-        <v>30</v>
+        <v>42</v>
+      </c>
+      <c r="R43" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -3287,46 +2941,40 @@
         <v>265</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>222</v>
+        <v>148</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>342</v>
+        <v>278</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>342</v>
+        <v>205</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="L44" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O44" s="4">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="P44" s="6" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
       <c r="Q44" s="9">
-        <v>63</v>
-      </c>
-      <c r="R44" s="9">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="R44" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -3334,43 +2982,46 @@
         <v>265</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>261</v>
+        <v>203</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>94</v>
+        <v>151</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>336</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="O45" s="4">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="P45" s="6" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="Q45" s="9">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="R45" s="9">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -3378,37 +3029,46 @@
         <v>265</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>37</v>
+        <v>153</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>38</v>
+        <v>279</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>262</v>
+        <v>246</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="M46" s="8" t="s">
-        <v>0</v>
+        <v>246</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="O46" s="4">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="P46" s="6" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="Q46" s="9">
-        <v>1</v>
-      </c>
-      <c r="R46" s="10" t="s">
-        <v>266</v>
+        <v>45</v>
+      </c>
+      <c r="R46" s="9">
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -3416,413 +3076,747 @@
         <v>265</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>263</v>
+        <v>108</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>263</v>
+        <v>247</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="J47" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="O47" s="4">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="Q47" s="9">
-        <v>2</v>
-      </c>
-      <c r="R47" s="10" t="s">
-        <v>266</v>
+        <v>46</v>
+      </c>
+      <c r="R47" s="9">
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
-        <v>265</v>
-      </c>
       <c r="B48" s="8" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
       <c r="F48" s="8"/>
       <c r="O48" s="4">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="P48" s="6" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="Q48" s="9">
-        <v>34</v>
-      </c>
-      <c r="R48" s="9">
-        <v>19</v>
+        <v>47</v>
+      </c>
+      <c r="R48" s="10" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B49" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
       <c r="F49" s="8"/>
       <c r="O49" s="4">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="P49" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q49" s="9">
         <v>48</v>
       </c>
-      <c r="Q49" s="9">
-        <v>6</v>
-      </c>
-      <c r="R49" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R49" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B50" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="F50" s="8"/>
+        <v>215</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="L50" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="O50" s="4">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="P50" s="6" t="s">
-        <v>46</v>
+        <v>160</v>
       </c>
       <c r="Q50" s="9">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="R50" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B51" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="F51" s="8"/>
+        <v>216</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="L51" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="O51" s="4">
+        <v>50</v>
+      </c>
+      <c r="P51" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q51" s="9">
+        <v>50</v>
+      </c>
+      <c r="R51" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L52" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="P51" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q51" s="9">
+      <c r="O52" s="4">
+        <v>51</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q52" s="9">
+        <v>51</v>
+      </c>
+      <c r="R52" s="9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O53" s="4">
+        <v>52</v>
+      </c>
+      <c r="P53" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q53" s="9">
+        <v>52</v>
+      </c>
+      <c r="R53" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="J54" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="R51" s="9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B52" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="O52" s="4">
-        <v>3</v>
-      </c>
-      <c r="P52" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q52" s="9">
-        <v>3</v>
-      </c>
-      <c r="R52" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B53" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="O53" s="4">
-        <v>30</v>
-      </c>
-      <c r="P53" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q53" s="9">
-        <v>30</v>
-      </c>
-      <c r="R53" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B54" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
       <c r="O54" s="4">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P54" s="6" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="Q54" s="9">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="R54" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B55" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
+        <v>176</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="O55" s="4">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="P55" s="6" t="s">
-        <v>62</v>
+        <v>175</v>
       </c>
       <c r="Q55" s="9">
-        <v>13</v>
-      </c>
-      <c r="R55" s="9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="R55" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B56" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
+        <v>179</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="O56" s="4">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="P56" s="6" t="s">
-        <v>50</v>
+        <v>178</v>
       </c>
       <c r="Q56" s="9">
-        <v>7</v>
-      </c>
-      <c r="R56" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="R56" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>265</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
+        <v>218</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>245</v>
+      </c>
       <c r="O57" s="4">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="P57" s="6" t="s">
-        <v>70</v>
+        <v>180</v>
       </c>
       <c r="Q57" s="9">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="R57" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B58" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
+        <v>219</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>338</v>
+      </c>
       <c r="O58" s="4">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="P58" s="6" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="Q58" s="9">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="R58" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B59" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
+        <v>183</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>340</v>
+      </c>
       <c r="O59" s="4">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="P59" s="6" t="s">
-        <v>66</v>
+        <v>182</v>
       </c>
       <c r="Q59" s="9">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="R59" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B60" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
+        <v>220</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="O60" s="4">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="P60" s="6" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="Q60" s="9">
-        <v>8</v>
-      </c>
-      <c r="R60" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="R60" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B61" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
+        <v>187</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>188</v>
+      </c>
       <c r="O61" s="4">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="P61" s="6" t="s">
-        <v>44</v>
+        <v>186</v>
       </c>
       <c r="Q61" s="9">
-        <v>4</v>
-      </c>
-      <c r="R61" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="R61" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B62" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
+        <v>221</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="H62" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="J62" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="L62" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="O62" s="4">
+        <v>61</v>
+      </c>
+      <c r="P62" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q62" s="9">
+        <v>61</v>
+      </c>
+      <c r="R62" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="L63" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="O63" s="4">
+        <v>62</v>
+      </c>
+      <c r="P63" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q63" s="9">
+        <v>62</v>
+      </c>
+      <c r="R63" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I64" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L64" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O64" s="4">
+        <v>63</v>
+      </c>
+      <c r="P64" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q64" s="9">
+        <v>63</v>
+      </c>
+      <c r="R64" s="9">
         <v>31</v>
       </c>
-      <c r="P62" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q62" s="9">
-        <v>31</v>
-      </c>
-      <c r="R62" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B63" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="O63" s="4">
-        <v>47</v>
-      </c>
-      <c r="P63" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q63" s="9">
-        <v>47</v>
-      </c>
-      <c r="R63" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B64" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="O64" s="4">
-        <v>16</v>
-      </c>
-      <c r="P64" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q64" s="9">
-        <v>16</v>
-      </c>
-      <c r="R64" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>265</v>
+      </c>
       <c r="B65" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
+        <v>195</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="H65" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="L65" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="O65" s="4">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="P65" s="6" t="s">
-        <v>73</v>
+        <v>194</v>
       </c>
       <c r="Q65" s="9">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="R65" s="9">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
@@ -4182,8 +4176,8 @@
       <c r="D97" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:U65">
-    <sortCondition ref="B2:B65"/>
+  <sortState ref="A2:R65">
+    <sortCondition ref="Q2:Q65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>